<commit_message>
Vilas da f up
</commit_message>
<xml_diff>
--- a/Entrega 2/DSS_2022-2023 - Use Case - alunos.xlsx
+++ b/Entrega 2/DSS_2022-2023 - Use Case - alunos.xlsx
@@ -5,23 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis-\Desktop\Universidade\LEI\3 Ano\DSS\GitHub\DSS2223\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmns2\Documents\GitHub\DSS2223\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B07C904-A4DA-461B-BC7E-F7F9F56898FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784D6C4A-97EC-4D77-9159-0B03045BD993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="2" r:id="rId1"/>
     <sheet name="3.1" sheetId="3" r:id="rId2"/>
+    <sheet name="3.4" sheetId="6" r:id="rId3"/>
+    <sheet name="3.6" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>1. Dividir os fluxos 
     em sequências de transacções</t>
@@ -124,6 +126,147 @@
   </si>
   <si>
     <t>Sistema informa administrador que já existe um campeonato com o mesmo nome</t>
+  </si>
+  <si>
+    <t>Criação de Pilotos</t>
+  </si>
+  <si>
+    <t>Um administrador cria um piloto</t>
+  </si>
+  <si>
+    <t>O André cria um piloto para os amigos</t>
+  </si>
+  <si>
+    <t>O utilizador autentica-se com conta de administrador</t>
+  </si>
+  <si>
+    <t>O piloto é criado e o sistema é atualizado</t>
+  </si>
+  <si>
+    <t>Administrador insere o nome, CTA, e SVA do piloto</t>
+  </si>
+  <si>
+    <t>O sistema guarda o piloto e atualiza</t>
+  </si>
+  <si>
+    <t>Sistema avisa sobre os valores inválidos</t>
+  </si>
+  <si>
+    <t>Inserir o nome, CTA e SVA</t>
+  </si>
+  <si>
+    <t>Configurar e simular corrida</t>
+  </si>
+  <si>
+    <t>Inicia-se a configuração das corridas do campeonato e posteriormente a simulação das mesmas</t>
+  </si>
+  <si>
+    <t>Como todos os amigos estão registados, o António decide começar a configuração para poder inicial a simulação</t>
+  </si>
+  <si>
+    <t>Pelo menos um campeonato configurado</t>
+  </si>
+  <si>
+    <t>Corrida simulada e pontuação atualizada para os jogadores autenticados</t>
+  </si>
+  <si>
+    <t>O jogador que configurou o campeonato inicia a configuração/simulação</t>
+  </si>
+  <si>
+    <t>As condições da corrida, o circuito inicial e a situação meteorológica são apresentadas aos utilizadores</t>
+  </si>
+  <si>
+    <t>Jogadores selecionam, se pretenderem, efetuar afinações, mudanças de pneu e/ou modo do motor</t>
+  </si>
+  <si>
+    <t>Sistema inicia a simulação, baseando-se nas posições relativas dos carros</t>
+  </si>
+  <si>
+    <t>Sistema apresenta, no final de cada volta, as posições dos jogadores</t>
+  </si>
+  <si>
+    <t>No final da corrida, o sistema apresenta as classificações de cada jogador</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>Todos os jogadores sofrem acidentes ou avarias (passo 5)</t>
+  </si>
+  <si>
+    <t>Valores CTS e/ou SVA inválidos (passo 1)</t>
+  </si>
+  <si>
+    <t>O sistema avisa que não há jogadores em condição para continuar (sem atribuição de pontos para esta corrida)</t>
+  </si>
+  <si>
+    <t>O sistema termina a corrida atual</t>
+  </si>
+  <si>
+    <t>Regressa a 8</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>Número de limite de afinações ultrapassado (passo 3)</t>
+  </si>
+  <si>
+    <t>Sistema avisa o limite ultrapassado de afinações (2/3 do número de corridas do campeonato)</t>
+  </si>
+  <si>
+    <t>Regressa a 6</t>
+  </si>
+  <si>
+    <t>"UI"</t>
+  </si>
+  <si>
+    <t>Efetuar afinações, mudanças de pneu e/ou modo do motor</t>
+  </si>
+  <si>
+    <t>public criaPiloto(nome:String, cta:Float, sva:Float):Piloto</t>
+  </si>
+  <si>
+    <t>Apresenta as classificações de cada jogador</t>
+  </si>
+  <si>
+    <t>public printClassificação():String</t>
+  </si>
+  <si>
+    <t>public efetuarAfinações(carro:Carro, downforce: Float, pneu:String, modoMotor:String): Carro</t>
+  </si>
+  <si>
+    <t>Sistema apresenta, durante a corrida,</t>
+  </si>
+  <si>
+    <t>eventuais despistes, avarias e/ou ultrapassagens ao longo do circuito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registar despistes, avarias e/ou ultrapassagens </t>
+  </si>
+  <si>
+    <t>public dnf(volta:Int, totalVoltas:Int, clime:Int): boolean</t>
+  </si>
+  <si>
+    <t>public simulaCorrida():Void { i=getVoltas()}</t>
   </si>
 </sst>
 </file>
@@ -278,6 +421,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
     </xf>
@@ -296,7 +440,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="45" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,104 +661,104 @@
       <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.6640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.33203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="7" width="43.33203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="8.6640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.44140625" style="1"/>
-    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.44140625" style="1"/>
+    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.6328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="7" width="43.36328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.453125" style="1"/>
+    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D1" s="2"/>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="2:10" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="22"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="2:10" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="22"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="22"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="22"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="22"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="22"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="2"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -625,7 +768,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -635,7 +778,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -645,7 +788,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -656,7 +799,7 @@
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="7"/>
@@ -664,7 +807,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -679,7 +822,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -689,7 +832,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="7"/>
@@ -697,7 +840,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -712,7 +855,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
@@ -723,32 +866,32 @@
       <c r="H18" s="8"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D27" s="2"/>
     </row>
   </sheetData>
@@ -772,40 +915,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946EE026-A836-1F45-848E-05AC37DD6D32}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68.77734375" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="68.81640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="54.44140625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="55.77734375" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.44140625" style="1"/>
-    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.44140625" style="1"/>
+    <col min="7" max="7" width="54.453125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="55.81640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.453125" style="1"/>
+    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="21" t="s">
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
@@ -813,12 +956,12 @@
       <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="22"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
@@ -826,67 +969,67 @@
       <c r="D3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="22"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="22"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="15"/>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="22"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="22"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="22"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15"/>
       <c r="C8" s="2"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
@@ -896,7 +1039,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="15"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
@@ -909,7 +1052,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="15"/>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -922,7 +1065,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="15"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -935,7 +1078,7 @@
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="15"/>
       <c r="C13" s="2"/>
       <c r="D13" s="12"/>
@@ -945,7 +1088,7 @@
       <c r="H13" s="8"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="15"/>
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
@@ -954,7 +1097,7 @@
       <c r="H14" s="8"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="15"/>
       <c r="C15" s="2"/>
       <c r="E15" s="8"/>
@@ -963,7 +1106,7 @@
       <c r="H15" s="8"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
@@ -973,7 +1116,7 @@
       <c r="H16" s="8"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
       <c r="C17" s="2"/>
       <c r="E17" s="7"/>
@@ -981,7 +1124,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="s">
         <v>13</v>
       </c>
@@ -992,7 +1135,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="15"/>
       <c r="C19" s="2"/>
       <c r="D19" s="17"/>
@@ -1001,7 +1144,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="15"/>
       <c r="C20" s="2"/>
       <c r="D20" s="17"/>
@@ -1010,7 +1153,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="15"/>
       <c r="C21" s="2"/>
       <c r="D21" s="17"/>
@@ -1019,7 +1162,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="15"/>
       <c r="C22" s="2"/>
       <c r="D22" s="17"/>
@@ -1028,7 +1171,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="15"/>
       <c r="C23" s="2"/>
       <c r="E23" s="7"/>
@@ -1036,7 +1179,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="15" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1194,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="15"/>
       <c r="C25" s="2" t="s">
         <v>30</v>
@@ -1065,7 +1208,7 @@
       <c r="H25" s="7"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="15"/>
       <c r="C26" s="5" t="s">
         <v>31</v>
@@ -1078,7 +1221,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="15"/>
       <c r="C27" s="5"/>
       <c r="D27" s="18"/>
@@ -1087,7 +1230,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="15"/>
       <c r="C28" s="20"/>
       <c r="D28" s="11"/>
@@ -1096,7 +1239,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="15"/>
       <c r="C29" s="2"/>
       <c r="D29" s="17"/>
@@ -1105,7 +1248,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="15"/>
       <c r="D30" s="17"/>
       <c r="E30" s="7"/>
@@ -1113,7 +1256,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="15"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1135,4 +1278,804 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C7EE73-6423-4A59-876C-ED9093227907}">
+  <dimension ref="B1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="68.81640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="56.54296875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="55.81640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.453125" style="1"/>
+    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.453125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="15"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="15"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="15"/>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="15"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="15"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="15"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="15"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="8"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="15"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="15"/>
+      <c r="C17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="15"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="15"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="15"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="15"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="15"/>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="15"/>
+      <c r="C26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="15"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="15"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="15"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="15"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E1:E8"/>
+    <mergeCell ref="F1:F8"/>
+    <mergeCell ref="G1:G8"/>
+    <mergeCell ref="H1:H8"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B18 B26:B28" xr:uid="{1F02A153-9DD9-406F-A6A3-F3312370207E}">
+      <formula1>"FLUXO DE EXCEÇÃO, FLUXO ALTERNATIVO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BB8140-56BE-4D68-86E7-4B85B4ACFB40}">
+  <dimension ref="B1:J31"/>
+  <sheetViews>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="111.81640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="95.81640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="55.81640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.453125" style="1"/>
+    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.453125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="15"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="15"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="15"/>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="15"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="15"/>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="15"/>
+      <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="15"/>
+      <c r="C14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="15"/>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="8"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="15"/>
+      <c r="C17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="15"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="15"/>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="15"/>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="15"/>
+      <c r="C22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="15"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="15"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="15"/>
+      <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="15"/>
+      <c r="C27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="15"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="15"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="15"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E1:E8"/>
+    <mergeCell ref="F1:F8"/>
+    <mergeCell ref="G1:G8"/>
+    <mergeCell ref="H1:H8"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25 B19 B27:B28" xr:uid="{779FE226-9EF8-4414-85FE-8B6B9095B34A}">
+      <formula1>"FLUXO DE EXCEÇÃO, FLUXO ALTERNATIVO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Falta 3.2 no excel ainda
</commit_message>
<xml_diff>
--- a/Entrega 2/DSS_2022-2023 - Use Case - alunos.xlsx
+++ b/Entrega 2/DSS_2022-2023 - Use Case - alunos.xlsx
@@ -5,29 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmns2\Documents\GitHub\DSS2223\Entrega 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis-\Desktop\Universidade\LEI\3 Ano\DSS\GitHub\DSS2223\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8C696C-F771-4728-8AF1-A056421FA7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD6F63B-FF44-4548-8284-ECB0067FDD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="2" r:id="rId1"/>
     <sheet name="3.1" sheetId="3" r:id="rId2"/>
     <sheet name="3.3" sheetId="7" r:id="rId3"/>
-    <sheet name="3.5" sheetId="9" r:id="rId4"/>
-    <sheet name="Folha3" sheetId="6" r:id="rId5"/>
-    <sheet name="3.7" sheetId="8" r:id="rId6"/>
-    <sheet name="3.4" sheetId="10" r:id="rId7"/>
-    <sheet name="3.6" sheetId="11" r:id="rId8"/>
+    <sheet name="3.4" sheetId="10" r:id="rId4"/>
+    <sheet name="3.5" sheetId="9" r:id="rId5"/>
+    <sheet name="3.6" sheetId="11" r:id="rId6"/>
+    <sheet name="3.7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="149">
   <si>
     <t>1. Dividir os fluxos 
     em sequências de transacções</t>
@@ -901,21 +900,21 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.6328125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="7" width="43.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="8.6328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="7" width="43.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.44140625" style="1"/>
+    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="2"/>
       <c r="E1" s="29" t="s">
         <v>0</v>
@@ -930,7 +929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -941,7 +940,7 @@
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="2:10" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
@@ -952,7 +951,7 @@
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -961,7 +960,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="29"/>
@@ -969,7 +968,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -979,7 +978,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -989,7 +988,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="5"/>
       <c r="E8" s="30"/>
@@ -998,7 +997,7 @@
       <c r="H8" s="34"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1008,7 +1007,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1018,7 +1017,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1027,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1039,7 +1038,7 @@
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="7"/>
@@ -1047,7 +1046,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1062,7 +1061,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1072,7 +1071,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="7"/>
@@ -1080,7 +1079,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1094,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1106,32 +1105,32 @@
       <c r="H18" s="8"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
     </row>
   </sheetData>
@@ -1159,22 +1158,22 @@
       <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="63.81640625" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.36328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="63.77734375" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.33203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="64" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="54.453125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="55.81640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1" collapsed="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
+    <col min="7" max="7" width="54.44140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="55.77734375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.44140625" style="1" collapsed="1"/>
+    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1200,7 @@
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
@@ -1214,7 +1213,7 @@
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1225,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
@@ -1235,7 +1234,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
@@ -1247,7 +1246,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
@@ -1259,7 +1258,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" s="2"/>
       <c r="D8" s="11"/>
@@ -1269,7 +1268,7 @@
       <c r="H8" s="34"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1278,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
@@ -1292,7 +1291,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" s="2" t="s">
         <v>34</v>
@@ -1305,7 +1304,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="2" t="s">
         <v>35</v>
@@ -1318,7 +1317,7 @@
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
       <c r="C13" s="2" t="s">
         <v>36</v>
@@ -1332,7 +1331,7 @@
       <c r="H13" s="8"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
@@ -1341,7 +1340,7 @@
       <c r="H14" s="8"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="2"/>
       <c r="E15" s="8"/>
@@ -1350,7 +1349,7 @@
       <c r="H15" s="8"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
@@ -1360,7 +1359,7 @@
       <c r="H16" s="8"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="2"/>
       <c r="E17" s="7"/>
@@ -1368,7 +1367,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
         <v>13</v>
       </c>
@@ -1379,7 +1378,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="2"/>
       <c r="D19" s="17"/>
@@ -1388,7 +1387,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="2"/>
       <c r="D20" s="17"/>
@@ -1397,7 +1396,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="2"/>
       <c r="D21" s="17"/>
@@ -1406,7 +1405,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="2"/>
       <c r="D22" s="17"/>
@@ -1415,7 +1414,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="2"/>
       <c r="E23" s="7"/>
@@ -1423,7 +1422,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
         <v>12</v>
       </c>
@@ -1438,7 +1437,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="2" t="s">
         <v>22</v>
@@ -1452,7 +1451,7 @@
       <c r="H25" s="7"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="5" t="s">
         <v>23</v>
@@ -1465,7 +1464,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="5"/>
       <c r="D27" s="18"/>
@@ -1474,7 +1473,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="15"/>
       <c r="C28" s="20"/>
       <c r="D28" s="11"/>
@@ -1483,7 +1482,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="2"/>
       <c r="D29" s="17"/>
@@ -1492,7 +1491,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="D30" s="17"/>
       <c r="E30" s="7"/>
@@ -1500,7 +1499,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1532,22 +1531,22 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="90.54296875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.36328125" style="27" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="43.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="71.6328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="38.81640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="90.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.33203125" style="27" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="43.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="71.6640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="38.77734375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.44140625" style="1"/>
+    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="2"/>
       <c r="E1" s="29" t="s">
         <v>0</v>
@@ -1562,7 +1561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1575,7 +1574,7 @@
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="2:10" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
@@ -1588,7 +1587,7 @@
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1600,7 +1599,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="29"/>
@@ -1608,7 +1607,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1620,7 +1619,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1631,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="5"/>
       <c r="E8" s="30"/>
@@ -1641,7 +1640,7 @@
       <c r="H8" s="34"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1651,7 +1650,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1665,7 +1664,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1677,7 +1676,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1692,7 +1691,7 @@
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>48</v>
       </c>
@@ -1704,7 +1703,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
         <v>50</v>
       </c>
@@ -1718,7 +1717,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>52</v>
       </c>
@@ -1729,7 +1728,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
@@ -1743,7 +1742,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="23"/>
@@ -1751,7 +1750,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1767,7 +1766,7 @@
       <c r="H18" s="8"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
@@ -1778,7 +1777,7 @@
       <c r="F19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1789,7 +1788,7 @@
       <c r="F20" s="7"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>60</v>
       </c>
@@ -1800,13 +1799,13 @@
       <c r="F21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
       <c r="E22" s="23"/>
       <c r="F22" s="7"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
@@ -1820,7 +1819,7 @@
       <c r="F23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1831,7 +1830,7 @@
       <c r="F24" s="7"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>38</v>
       </c>
@@ -1842,7 +1841,7 @@
       <c r="F25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
@@ -1853,13 +1852,13 @@
       <c r="F26" s="7"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
       <c r="E27" s="24"/>
       <c r="F27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1873,7 +1872,7 @@
       <c r="F28" s="7"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1884,7 +1883,7 @@
       <c r="F29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1895,7 +1894,7 @@
       <c r="F30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1906,7 +1905,7 @@
       <c r="F31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>69</v>
       </c>
@@ -1917,7 +1916,7 @@
       <c r="F32" s="7"/>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>70</v>
       </c>
@@ -1928,12 +1927,12 @@
       <c r="F33" s="7"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="2:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="24"/>
       <c r="F34" s="7"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
@@ -1947,7 +1946,7 @@
       <c r="F35" s="7"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1958,7 +1957,7 @@
       <c r="F36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>38</v>
       </c>
@@ -1969,7 +1968,7 @@
       <c r="F37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>60</v>
       </c>
@@ -1980,7 +1979,7 @@
       <c r="F38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>69</v>
       </c>
@@ -1991,7 +1990,7 @@
       <c r="F39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="2:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>70</v>
       </c>
@@ -2002,7 +2001,7 @@
       <c r="F40" s="7"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>75</v>
       </c>
@@ -2013,12 +2012,12 @@
       <c r="F41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E42" s="24"/>
       <c r="F42" s="7"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
@@ -2032,7 +2031,7 @@
       <c r="F43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>34</v>
       </c>
@@ -2043,7 +2042,7 @@
       <c r="F44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>38</v>
       </c>
@@ -2054,7 +2053,7 @@
       <c r="F45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>60</v>
       </c>
@@ -2065,12 +2064,12 @@
       <c r="F46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E47" s="24"/>
       <c r="F47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>13</v>
       </c>
@@ -2084,7 +2083,7 @@
       <c r="F48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>34</v>
       </c>
@@ -2095,7 +2094,7 @@
       <c r="F49" s="7"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>38</v>
       </c>
@@ -2106,7 +2105,7 @@
       <c r="F50" s="7"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>60</v>
       </c>
@@ -2117,7 +2116,7 @@
       <c r="F51" s="7"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
         <v>69</v>
       </c>
@@ -2128,7 +2127,7 @@
       <c r="F52" s="7"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>70</v>
       </c>
@@ -2139,12 +2138,12 @@
       <c r="F53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E54" s="24"/>
       <c r="F54" s="7"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>84</v>
       </c>
@@ -2158,7 +2157,7 @@
       <c r="F55" s="7"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>22</v>
       </c>
@@ -2169,7 +2168,7 @@
       <c r="F56" s="7"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
         <v>23</v>
       </c>
@@ -2180,12 +2179,12 @@
       <c r="F57" s="7"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E58" s="24"/>
       <c r="F58" s="7"/>
       <c r="H58" s="7"/>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>84</v>
       </c>
@@ -2199,7 +2198,7 @@
       <c r="F59" s="7"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C60" s="1" t="s">
         <v>22</v>
       </c>
@@ -2210,7 +2209,7 @@
       <c r="F60" s="7"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
         <v>23</v>
       </c>
@@ -2221,12 +2220,12 @@
       <c r="F61" s="7"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E62" s="24"/>
       <c r="F62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>84</v>
       </c>
@@ -2240,7 +2239,7 @@
       <c r="F63" s="7"/>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
         <v>88</v>
       </c>
@@ -2251,7 +2250,7 @@
       <c r="F64" s="7"/>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
         <v>89</v>
       </c>
@@ -2262,12 +2261,12 @@
       <c r="F65" s="7"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E66" s="24"/>
       <c r="F66" s="7"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>84</v>
       </c>
@@ -2280,7 +2279,7 @@
       <c r="E67" s="24"/>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
         <v>22</v>
       </c>
@@ -2290,7 +2289,7 @@
       <c r="E68" s="24"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
         <v>23</v>
       </c>
@@ -2300,11 +2299,11 @@
       <c r="E69" s="24"/>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E70" s="24"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
         <v>84</v>
       </c>
@@ -2317,7 +2316,7 @@
       <c r="E71" s="24"/>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
         <v>92</v>
       </c>
@@ -2327,7 +2326,7 @@
       <c r="E72" s="24"/>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
         <v>93</v>
       </c>
@@ -2337,11 +2336,11 @@
       <c r="E73" s="24"/>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E74" s="24"/>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="2:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:8" ht="30" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
         <v>84</v>
       </c>
@@ -2354,7 +2353,7 @@
       <c r="E75" s="24"/>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C76" s="1" t="s">
         <v>96</v>
       </c>
@@ -2364,7 +2363,7 @@
       <c r="E76" s="24"/>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C77" s="1" t="s">
         <v>98</v>
       </c>
@@ -2374,383 +2373,383 @@
       <c r="E77" s="24"/>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E78" s="24"/>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E79" s="24"/>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E80" s="24"/>
       <c r="F80" s="7"/>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" s="24"/>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E82" s="24"/>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E83" s="24"/>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E84" s="24"/>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E85" s="24"/>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E86" s="24"/>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E87" s="24"/>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E88" s="24"/>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E89" s="24"/>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E90" s="24"/>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E91" s="24"/>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E92" s="24"/>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E93" s="24"/>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E94" s="24"/>
     </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E95" s="24"/>
     </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E96" s="24"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="24"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="24"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="24"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="24"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="24"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="24"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="24"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="24"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="24"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="24"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="24"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="24"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="24"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="24"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="24"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="24"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="24"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="24"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="24"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="24"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="24"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="24"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="24"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="24"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="24"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="24"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="24"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="24"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="24"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" s="24"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" s="24"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" s="24"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="24"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="24"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="24"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="24"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="24"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="24"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="24"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="24"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="24"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="24"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="24"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="24"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="24"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="24"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="24"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="24"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="24"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="24"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="24"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="24"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="24"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="24"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="24"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" s="24"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" s="24"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E154" s="24"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E155" s="24"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E156" s="24"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E157" s="24"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" s="24"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E159" s="24"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E160" s="24"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E161" s="24"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E162" s="24"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E163" s="24"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E164" s="24"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E165" s="24"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E166" s="24"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E167" s="24"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E168" s="24"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E169" s="24"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E170" s="24"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E171" s="24"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E172" s="24"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E173" s="24"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E174" s="24"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E175" s="24"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E176" s="24"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E177" s="24"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E178" s="24"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E179" s="24"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E180" s="24"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E181" s="24"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E182" s="24"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E183" s="24"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E184" s="24"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E185" s="24"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E186" s="24"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E187" s="24"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E188" s="24"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E189" s="24"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E190" s="24"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E191" s="24"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E192" s="24"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E193" s="24"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E194" s="24"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E195" s="24"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E196" s="24"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E197" s="24"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E198" s="24"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E199" s="24"/>
     </row>
   </sheetData>
@@ -2770,6 +2769,376 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60ADBABA-F9E9-4362-868A-08B88E53357D}">
+  <dimension ref="B1:J31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="68.77734375" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="56.5546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="55.77734375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.44140625" style="1"/>
+    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="15"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="8"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="15"/>
+      <c r="C26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="15"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="15"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="15"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E1:E8"/>
+    <mergeCell ref="F1:F8"/>
+    <mergeCell ref="G1:G8"/>
+    <mergeCell ref="H1:H8"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B18 B26:B28" xr:uid="{21B10A29-F849-49BF-9FD5-18CDC197571F}">
+      <formula1>"FLUXO DE EXCEÇÃO, FLUXO ALTERNATIVO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F81F3E-6469-4057-A5EB-56DD19FE973F}">
   <dimension ref="B1:J199"/>
   <sheetViews>
@@ -2777,22 +3146,22 @@
       <selection activeCell="B15" sqref="B15:D88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="58" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.36328125" style="27" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="43.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="71.6328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="38.81640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
+    <col min="5" max="5" width="20.33203125" style="27" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="43.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="71.6640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="38.77734375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.44140625" style="1"/>
+    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="2"/>
       <c r="E1" s="29" t="s">
         <v>0</v>
@@ -2807,7 +3176,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2820,7 +3189,7 @@
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="2:10" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
@@ -2833,7 +3202,7 @@
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2845,7 +3214,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="29"/>
@@ -2853,7 +3222,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2865,7 +3234,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2877,7 +3246,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="5"/>
       <c r="E8" s="30"/>
@@ -2886,7 +3255,7 @@
       <c r="H8" s="34"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -2896,7 +3265,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2908,7 +3277,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2920,7 +3289,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2933,7 +3302,7 @@
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>48</v>
       </c>
@@ -2945,7 +3314,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="5"/>
       <c r="E14" s="23"/>
@@ -2953,14 +3322,14 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="25"/>
       <c r="D15" s="2"/>
       <c r="E15" s="24"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="23"/>
@@ -2968,14 +3337,14 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
       <c r="E17" s="23"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
       <c r="E18" s="24"/>
       <c r="F18" s="7"/>
@@ -2983,695 +3352,695 @@
       <c r="H18" s="8"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="2"/>
       <c r="E19" s="24"/>
       <c r="F19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="24"/>
       <c r="F20" s="7"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
       <c r="E21" s="24"/>
       <c r="F21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
       <c r="E22" s="23"/>
       <c r="F22" s="7"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="2"/>
       <c r="E23" s="23"/>
       <c r="F23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="2"/>
       <c r="E24" s="24"/>
       <c r="F24" s="7"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="3"/>
       <c r="E25" s="24"/>
       <c r="F25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="24"/>
       <c r="F26" s="7"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="24"/>
       <c r="F27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E28" s="24"/>
       <c r="F28" s="7"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E29" s="24"/>
       <c r="F29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E30" s="24"/>
       <c r="F30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E31" s="24"/>
       <c r="F31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C32" s="3"/>
       <c r="E32" s="24"/>
       <c r="F32" s="7"/>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E33" s="24"/>
       <c r="F33" s="7"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="3:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="24"/>
       <c r="F34" s="7"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E35" s="24"/>
       <c r="F35" s="7"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E36" s="24"/>
       <c r="F36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E37" s="24"/>
       <c r="F37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E38" s="24"/>
       <c r="F38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E39" s="24"/>
       <c r="F39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="3:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3"/>
       <c r="D40" s="2"/>
       <c r="E40" s="24"/>
       <c r="F40" s="7"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D41" s="2"/>
       <c r="E41" s="24"/>
       <c r="F41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D42" s="2"/>
       <c r="E42" s="24"/>
       <c r="F42" s="7"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D43" s="2"/>
       <c r="E43" s="24"/>
       <c r="F43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E44" s="24"/>
       <c r="F44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
       <c r="D45" s="2"/>
       <c r="E45" s="24"/>
       <c r="F45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E46" s="24"/>
       <c r="F46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D47" s="2"/>
       <c r="E47" s="24"/>
       <c r="F47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D48" s="2"/>
       <c r="E48" s="24"/>
       <c r="F48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D49" s="2"/>
       <c r="E49" s="24"/>
       <c r="F49" s="7"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E50" s="24"/>
       <c r="F50" s="7"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E51" s="24"/>
       <c r="F51" s="7"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C52" s="3"/>
       <c r="E52" s="24"/>
       <c r="F52" s="7"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E53" s="24"/>
       <c r="F53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E54" s="24"/>
       <c r="F54" s="7"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E55" s="24"/>
       <c r="F55" s="7"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C56" s="3"/>
       <c r="E56" s="24"/>
       <c r="F56" s="7"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E57" s="24"/>
       <c r="F57" s="7"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E58" s="24"/>
       <c r="F58" s="7"/>
       <c r="H58" s="7"/>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E59" s="24"/>
       <c r="F59" s="7"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C60" s="3"/>
       <c r="E60" s="24"/>
       <c r="F60" s="7"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E61" s="24"/>
       <c r="F61" s="7"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E62" s="24"/>
       <c r="F62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E63" s="24"/>
       <c r="F63" s="7"/>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C64" s="3"/>
       <c r="D64" s="26"/>
       <c r="E64" s="24"/>
       <c r="F64" s="7"/>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E65" s="24"/>
       <c r="F65" s="7"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E66" s="24"/>
       <c r="F66" s="7"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E67" s="24"/>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C68" s="3"/>
       <c r="D68" s="26"/>
       <c r="E68" s="24"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E69" s="24"/>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E70" s="24"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E71" s="24"/>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C72" s="3"/>
       <c r="D72" s="26"/>
       <c r="E72" s="24"/>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E73" s="24"/>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E74" s="24"/>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E75" s="24"/>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E76" s="24"/>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E77" s="24"/>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E78" s="24"/>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E79" s="24"/>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E80" s="24"/>
       <c r="F80" s="7"/>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" s="24"/>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E82" s="24"/>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E83" s="24"/>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E84" s="24"/>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E85" s="24"/>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E86" s="24"/>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E87" s="24"/>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E88" s="24"/>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E89" s="24"/>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E90" s="24"/>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E91" s="24"/>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E92" s="24"/>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E93" s="24"/>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E94" s="24"/>
     </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E95" s="24"/>
     </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E96" s="24"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="24"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="24"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="24"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="24"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="24"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="24"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="24"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="24"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="24"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="24"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="24"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="24"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="24"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="24"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="24"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="24"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="24"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="24"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="24"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="24"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="24"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="24"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="24"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="24"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="24"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="24"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="24"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="24"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="24"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" s="24"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" s="24"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" s="24"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="24"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="24"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="24"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="24"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="24"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="24"/>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="24"/>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="24"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="24"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="24"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="24"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="24"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="24"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="24"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="24"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="24"/>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="24"/>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="24"/>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="24"/>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="24"/>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="24"/>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="24"/>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="24"/>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" s="24"/>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" s="24"/>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E154" s="24"/>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E155" s="24"/>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E156" s="24"/>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E157" s="24"/>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" s="24"/>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E159" s="24"/>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E160" s="24"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E161" s="24"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E162" s="24"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E163" s="24"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E164" s="24"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E165" s="24"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E166" s="24"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E167" s="24"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E168" s="24"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E169" s="24"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E170" s="24"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E171" s="24"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E172" s="24"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E173" s="24"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E174" s="24"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E175" s="24"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E176" s="24"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E177" s="24"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E178" s="24"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E179" s="24"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E180" s="24"/>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E181" s="24"/>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E182" s="24"/>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E183" s="24"/>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E184" s="24"/>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E185" s="24"/>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E186" s="24"/>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E187" s="24"/>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E188" s="24"/>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E189" s="24"/>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E190" s="24"/>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E191" s="24"/>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E192" s="24"/>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E193" s="24"/>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E194" s="24"/>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E195" s="24"/>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E196" s="24"/>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E197" s="24"/>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E198" s="24"/>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E199" s="24"/>
     </row>
   </sheetData>
@@ -3691,30 +4060,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3371FC30-3CF6-4049-A8B8-2134D29DBAE6}">
-  <dimension ref="B1:J27"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4E9E3B-E10F-440E-84CF-5CAF592A51B7}">
+  <dimension ref="B1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.6328125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="7" width="43.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="8.6328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="111.77734375" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="95.77734375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="55.77734375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.44140625" style="1"/>
+    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="2"/>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
@@ -3728,45 +4097,46 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="32"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="2:10" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="10" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="E3" s="29"/>
       <c r="F3" s="32"/>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:10" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="32"/>
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="15"/>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="29"/>
@@ -3774,178 +4144,334 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
+      <c r="D6" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="32"/>
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
+      <c r="D7" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="32"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="30"/>
       <c r="F8" s="33"/>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>31</v>
+      <c r="D10" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
       <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
       <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
       <c r="C13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="8"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
+      <c r="C19" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="2"/>
+      <c r="C25" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="15"/>
+      <c r="C26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="15"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="15"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="15"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3955,7 +4481,7 @@
     <mergeCell ref="H1:H8"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17 B14 B19" xr:uid="{0BD847B6-46CC-B445-85B7-E4F991ED5BFF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25 B19 B27:B28" xr:uid="{4D9FAE94-B8D3-417D-AD5D-ECF7531DE62C}">
       <formula1>"FLUXO DE EXCEÇÃO, FLUXO ALTERNATIVO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3963,30 +4489,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07C38FC-7B62-4793-A839-B5FC3B457BC5}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68.81640625" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="68.77734375" style="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.33203125" style="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="54.453125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="55.81640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
+    <col min="7" max="7" width="54.44140625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="55.77734375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.44140625" style="1"/>
+    <col min="10" max="10" width="53.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
@@ -4013,7 +4539,7 @@
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
@@ -4026,7 +4552,7 @@
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
@@ -4036,7 +4562,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
@@ -4045,7 +4571,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
@@ -4057,7 +4583,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
@@ -4069,7 +4595,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" s="2"/>
       <c r="D8" s="11"/>
@@ -4079,7 +4605,7 @@
       <c r="H8" s="34"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
@@ -4089,7 +4615,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="2" t="s">
         <v>8</v>
@@ -4106,7 +4632,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -4121,7 +4647,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="2" t="s">
         <v>9</v>
@@ -4134,7 +4660,7 @@
       <c r="H12" s="8"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="C13" s="2"/>
       <c r="D13" s="12"/>
@@ -4144,7 +4670,7 @@
       <c r="H13" s="8"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
@@ -4153,7 +4679,7 @@
       <c r="H14" s="8"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="2"/>
       <c r="E15" s="8"/>
@@ -4162,7 +4688,7 @@
       <c r="H15" s="8"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
@@ -4172,7 +4698,7 @@
       <c r="H16" s="8"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="2"/>
       <c r="E17" s="7"/>
@@ -4180,7 +4706,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="15"/>
       <c r="C18" s="19"/>
       <c r="D18" s="11"/>
@@ -4189,7 +4715,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="2"/>
       <c r="D19" s="17"/>
@@ -4198,7 +4724,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="2"/>
       <c r="D20" s="17"/>
@@ -4207,7 +4733,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="2"/>
       <c r="D21" s="17"/>
@@ -4216,7 +4742,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="2"/>
       <c r="D22" s="17"/>
@@ -4225,7 +4751,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="2"/>
       <c r="E23" s="7"/>
@@ -4233,7 +4759,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="15"/>
       <c r="C24" s="20"/>
       <c r="D24" s="11"/>
@@ -4242,7 +4768,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="2"/>
       <c r="D25" s="17"/>
@@ -4252,7 +4778,7 @@
       <c r="H25" s="7"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="5"/>
       <c r="D26" s="18"/>
@@ -4261,7 +4787,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="5"/>
       <c r="D27" s="18"/>
@@ -4270,7 +4796,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="15"/>
       <c r="C28" s="20"/>
       <c r="D28" s="11"/>
@@ -4279,7 +4805,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="2"/>
       <c r="D29" s="17"/>
@@ -4288,7 +4814,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="D30" s="17"/>
       <c r="E30" s="7"/>
@@ -4296,7 +4822,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -4317,803 +4843,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60ADBABA-F9E9-4362-868A-08B88E53357D}">
-  <dimension ref="B1:J31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68.81640625" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="56.54296875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="55.81640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="15"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="15"/>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="15"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="15"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="15"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="8"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="15"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="15"/>
-      <c r="C17" s="2"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B18" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="15"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="15"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="15"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="2"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B25" s="15"/>
-      <c r="C25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B26" s="15"/>
-      <c r="C26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="15"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="15"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B29" s="15"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B30" s="15"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B31" s="15"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E1:E8"/>
-    <mergeCell ref="F1:F8"/>
-    <mergeCell ref="G1:G8"/>
-    <mergeCell ref="H1:H8"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B18 B26:B28" xr:uid="{21B10A29-F849-49BF-9FD5-18CDC197571F}">
-      <formula1>"FLUXO DE EXCEÇÃO, FLUXO ALTERNATIVO"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4E9E3B-E10F-440E-84CF-5CAF592A51B7}">
-  <dimension ref="B1:J31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="1.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="111.81640625" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.36328125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="64" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="95.81640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="55.81640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.453125" style="1"/>
-    <col min="10" max="10" width="53.453125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.453125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="15"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="15"/>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="15"/>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
-      <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="15"/>
-      <c r="C14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D15" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="15"/>
-      <c r="C16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="8"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="15"/>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B18" s="15"/>
-      <c r="C18" s="2"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="15"/>
-      <c r="C20" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
-      <c r="C21" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="15"/>
-      <c r="C22" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24" s="15"/>
-      <c r="C24" s="2"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B25" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B26" s="15"/>
-      <c r="C26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="15"/>
-      <c r="C27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="15"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B29" s="15"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B30" s="15"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B31" s="15"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E1:E8"/>
-    <mergeCell ref="F1:F8"/>
-    <mergeCell ref="G1:G8"/>
-    <mergeCell ref="H1:H8"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25 B19 B27:B28" xr:uid="{4D9FAE94-B8D3-417D-AD5D-ECF7531DE62C}">
-      <formula1>"FLUXO DE EXCEÇÃO, FLUXO ALTERNATIVO"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>